<commit_message>
DSA 450: 5 Question Solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Software Engineer\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953A380B-0BE9-4A8D-AFFD-78F62D94C2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC0FD66-895E-4252-823D-6F0C43D2A60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -1949,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1960,7 +1960,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1971,7 +1971,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1982,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -1993,7 +1993,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 4 Questions
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Software Engineer\Data-Structure-Algorithm-Module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC0FD66-895E-4252-823D-6F0C43D2A60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F9373B-6848-49AA-97C0-FBBB92255BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="360" yWindow="570" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2015,7 +2015,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2026,7 +2026,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2037,7 +2037,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2048,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 2 Questions
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F9373B-6848-49AA-97C0-FBBB92255BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D555BE7F-BFF5-4AA8-BF7C-71A251BFE610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="570" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2059,7 +2059,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: Question -2
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D555BE7F-BFF5-4AA8-BF7C-71A251BFE610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FC9F28-E0F6-43A9-8C20-F06E2EFD3A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="570" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1861,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2070,7 +2064,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2081,7 +2075,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2092,7 +2086,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 2 Questions of Subarray Solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6310C3-8AD2-4F3C-BF73-3171728E35EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313B9090-182C-41F9-8DC5-4EF00A2E04E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="570" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2130,7 +2130,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21">
@@ -2141,7 +2141,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 3 Questions solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313B9090-182C-41F9-8DC5-4EF00A2E04E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5E0EA5-6883-4CC0-AB2C-88C0E78E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2152,7 +2152,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
@@ -2163,7 +2163,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2174,7 +2174,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 3 qquestion solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5E0EA5-6883-4CC0-AB2C-88C0E78E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8720AED8-EB20-46C7-AFCF-19570F20ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2185,7 +2185,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">
@@ -2196,7 +2196,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 2 Question Solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8720AED8-EB20-46C7-AFCF-19570F20ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AADD3F-589E-4106-B1F5-B2A923B137EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2207,7 +2207,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -2218,7 +2218,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 2 questions solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AADD3F-589E-4106-B1F5-B2A923B137EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A7BA5-5EE0-47E4-85A0-D7ABAC0ED9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2229,7 +2229,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2240,7 +2240,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 4 Question Solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A7BA5-5EE0-47E4-85A0-D7ABAC0ED9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6775523-B147-4B66-A298-7DCAE068DE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2251,7 +2251,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2262,7 +2262,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2273,7 +2273,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2284,7 +2284,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 1 matrix question Solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6775523-B147-4B66-A298-7DCAE068DE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEB6BA1-0C1E-4DEE-86BB-257AE13CE06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2308,7 +2308,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 3 questions solved 2 questions later
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63031051-414D-43F7-B6AC-CA3FB3DF9514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581D964A-D8F4-42B0-9422-22056B9B34DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1425,7 +1425,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Half</t>
+    <t>Not Understand the Questions</t>
   </si>
 </sst>
 </file>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2366,7 +2366,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>466</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21">
@@ -2377,7 +2377,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">
@@ -2388,7 +2388,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="21">
@@ -2399,7 +2399,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="21">
@@ -2410,7 +2410,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 5 question solved + 1 theory question
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581D964A-D8F4-42B0-9422-22056B9B34DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209E3FEB-219C-4E93-9015-5ACA196435AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="5295" yWindow="1920" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="B54" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2426,7 +2426,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
@@ -2437,7 +2437,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">
@@ -2448,7 +2448,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="21">
@@ -2459,7 +2459,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21">
@@ -2470,7 +2470,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21">
@@ -2481,7 +2481,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 1 question Solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209E3FEB-219C-4E93-9015-5ACA196435AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC35B64A-DBB2-4096-9E2D-78856DFC5377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="1920" windowWidth="21600" windowHeight="11295" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B54" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2492,7 +2492,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 1 question solved and Learning Dynamic programming concept
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC35B64A-DBB2-4096-9E2D-78856DFC5377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF07AACC-BFFE-498A-869E-D29B70937658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t>Not Understand the Questions</t>
+  </si>
+  <si>
+    <t>Learning Dynamic Programming</t>
   </si>
 </sst>
 </file>
@@ -1857,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2503,7 +2506,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21">
@@ -2514,7 +2517,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: Dynamic Programming
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF07AACC-BFFE-498A-869E-D29B70937658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551154AD-7FDC-4245-8E0C-64BC29B1AF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,9 +1426,6 @@
   </si>
   <si>
     <t>Not Understand the Questions</t>
-  </si>
-  <si>
-    <t>Learning Dynamic Programming</t>
   </si>
 </sst>
 </file>
@@ -1861,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2517,7 +2514,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -2528,7 +2525,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21">
@@ -2538,9 +2535,7 @@
       <c r="B66" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C66" s="4"/>
     </row>
     <row r="67" spans="1:3" ht="21">
       <c r="A67" s="5" t="s">

</xml_diff>

<commit_message>
DSA 460: Permutation of a String
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551154AD-7FDC-4245-8E0C-64BC29B1AF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1000E-0D32-4CB8-A2CB-3F10DA43CAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2535,7 +2535,9 @@
       <c r="B66" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="4"/>
+      <c r="C66" s="4" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="67" spans="1:3" ht="21">
       <c r="A67" s="5" t="s">

</xml_diff>

<commit_message>
DSA 460: 1 question solved now focusing on learning dynamic programmming
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1000E-0D32-4CB8-A2CB-3F10DA43CAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF131C-A3A1-4FE8-9D27-45F5007AA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2547,7 +2547,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: Dynamic Programming implementation
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF131C-A3A1-4FE8-9D27-45F5007AA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3CE614-7D73-49DF-BC96-E63A6F57125A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="B399" workbookViewId="0">
+      <selection activeCell="G413" sqref="G413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6157,7 +6157,7 @@
         <v>394</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
@@ -6168,7 +6168,7 @@
         <v>395</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
@@ -6179,7 +6179,7 @@
         <v>396</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6223,7 +6223,7 @@
         <v>400</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 2 question of DP solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3CE614-7D73-49DF-BC96-E63A6F57125A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB9C758-3030-4DB2-B014-9F37C123F79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B399" workbookViewId="0">
-      <selection activeCell="G413" sqref="G413"/>
+    <sheetView tabSelected="1" topLeftCell="B411" workbookViewId="0">
+      <selection activeCell="C423" sqref="C423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6234,7 +6234,7 @@
         <v>273</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="21">
@@ -6300,7 +6300,7 @@
         <v>406</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: Tried programmming challange + Solved Basics questions
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB9C758-3030-4DB2-B014-9F37C123F79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27164CA-9BAD-48C6-8365-C855DC1D4BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B411" workbookViewId="0">
-      <selection activeCell="C423" sqref="C423"/>
+    <sheetView tabSelected="1" topLeftCell="B405" workbookViewId="0">
+      <selection activeCell="C413" sqref="C413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6190,7 +6190,7 @@
         <v>397</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="21">
@@ -6201,7 +6201,7 @@
         <v>398</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 2 questions of DP Implementation
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27164CA-9BAD-48C6-8365-C855DC1D4BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3052DB82-F384-4688-A9E0-644FDCCDBB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B405" workbookViewId="0">
-      <selection activeCell="C413" sqref="C413"/>
+    <sheetView tabSelected="1" topLeftCell="B408" workbookViewId="0">
+      <selection activeCell="C419" sqref="C419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6245,7 +6245,7 @@
         <v>401</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="21">
@@ -6256,7 +6256,7 @@
         <v>402</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: Restarted with two questions
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3052DB82-F384-4688-A9E0-644FDCCDBB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6BDC16-EAF9-4041-B2AF-0A57E685DA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="600" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B408" workbookViewId="0">
-      <selection activeCell="C419" sqref="C419"/>
+    <sheetView tabSelected="1" topLeftCell="B414" workbookViewId="0">
+      <selection activeCell="C423" sqref="C423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6267,7 +6267,7 @@
         <v>403</v>
       </c>
       <c r="C420" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="421" spans="1:3" ht="21">
@@ -6278,7 +6278,7 @@
         <v>404</v>
       </c>
       <c r="C421" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: 4 Questions solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570B9FC1-41D9-4A1F-8929-1159C976884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2926FD8E-12D5-485C-A024-475C9B3FB79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="2985" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t>Not Understand the Questions</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1857,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C417" workbookViewId="0">
-      <selection activeCell="D425" sqref="D425"/>
+    <sheetView tabSelected="1" topLeftCell="C411" workbookViewId="0">
+      <selection activeCell="C432" sqref="C432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6355,7 +6358,7 @@
         <v>411</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="21">
@@ -6366,7 +6369,7 @@
         <v>412</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="21">
@@ -6377,7 +6380,7 @@
         <v>413</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="21">
@@ -6388,7 +6391,7 @@
         <v>414</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="432" spans="1:3" ht="21">
@@ -6398,9 +6401,7 @@
       <c r="B432" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="C432" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C432" s="4"/>
     </row>
     <row r="433" spans="1:3" ht="21">
       <c r="A433" s="5" t="s">

</xml_diff>

<commit_message>
DSA 460: 1 question started + Linkelist Concepts
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2926FD8E-12D5-485C-A024-475C9B3FB79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CBBB7F-6585-43D0-ADCE-60FC811B8A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="2985" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C411" workbookViewId="0">
-      <selection activeCell="C432" sqref="C432"/>
+    <sheetView tabSelected="1" topLeftCell="C417" workbookViewId="0">
+      <selection activeCell="D432" sqref="D432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6401,7 +6401,9 @@
       <c r="B432" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="C432" s="4"/>
+      <c r="C432" s="4" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="433" spans="1:3" ht="21">
       <c r="A433" s="5" t="s">

</xml_diff>

<commit_message>
DSA 460: Linked List 4 question solved and understanding concept
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CBBB7F-6585-43D0-ADCE-60FC811B8A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C43A0A1-4C18-4897-9648-85AE843611A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="2985" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C417" workbookViewId="0">
-      <selection activeCell="D432" sqref="D432"/>
+    <sheetView tabSelected="1" topLeftCell="C131" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -3307,7 +3307,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3318,7 +3318,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
@@ -3329,7 +3329,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3351,7 +3351,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">

</xml_diff>

<commit_message>
DSA 460: Linked List 4 question solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Data-Structure-Algorithm-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C43A0A1-4C18-4897-9648-85AE843611A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8569C70C-780B-40B6-B8D5-49B1C5350C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="2985" windowWidth="21630" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1850,7 +1850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C131" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="C134" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -3362,7 +3362,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3373,7 +3373,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
@@ -3384,7 +3384,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">
@@ -3395,7 +3395,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">

</xml_diff>